<commit_message>
add more to data set
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Third year 2nd semester\Perfomance Modelling\mini project\Performance-Modelling-Mini-Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9E55C-9E72-4E2C-9C95-A2F62E54E0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="74">
   <si>
     <t>Test ID</t>
   </si>
@@ -220,12 +226,30 @@
   </si>
   <si>
     <t>High time</t>
+  </si>
+  <si>
+    <t>Thelakataha Gaatha</t>
+  </si>
+  <si>
+    <t>9.0.98.1187</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Bones</t>
+  </si>
+  <si>
+    <t>Ape gam gode</t>
+  </si>
+  <si>
+    <t>Demons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,15 +288,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -284,14 +308,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -329,7 +356,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -401,7 +428,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -574,11 +601,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,8 +617,8 @@
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -626,10 +653,10 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L1" t="s">
@@ -679,10 +706,10 @@
       <c r="I2">
         <v>3.87</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>54.29</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="L2" t="s">
@@ -732,10 +759,10 @@
       <c r="I3">
         <v>2.3199999999999998</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>70.42</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>49</v>
       </c>
       <c r="L3" t="s">
@@ -785,10 +812,10 @@
       <c r="I4">
         <v>3.68</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>62.49</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>49</v>
       </c>
       <c r="L4" t="s">
@@ -838,10 +865,10 @@
       <c r="I5">
         <v>1.75</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>67.69</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="L5" t="s">
@@ -891,7 +918,7 @@
       <c r="I6" s="2">
         <v>16.8</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>50.31</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -944,7 +971,7 @@
       <c r="I7" s="2">
         <v>0.06</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>151.69</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -997,7 +1024,7 @@
       <c r="I8" s="2">
         <v>9.2100000000000009</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>62.44</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1050,7 +1077,7 @@
       <c r="I9" s="2">
         <v>1.62</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>58.64</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1082,129 +1109,309 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="2"/>
+      <c r="C10" s="3">
+        <v>45994.413888888892</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10.7</v>
+      </c>
+      <c r="J10" s="6">
+        <v>153.595</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10">
+        <v>310</v>
+      </c>
+      <c r="O10">
+        <v>1.88</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="2"/>
+      <c r="C11" s="3">
+        <v>45994.427083333336</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="J11" s="7">
+        <v>382.79500000000002</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11">
+        <v>165</v>
+      </c>
+      <c r="O11">
+        <v>0.98</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="2"/>
+      <c r="C12" s="3">
+        <v>45994.46875</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="J12" s="6">
+        <v>270.464</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12">
+        <v>327</v>
+      </c>
+      <c r="O12">
+        <v>1.55</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="2"/>
+      <c r="C13" s="3">
+        <v>45994.479166666664</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="J13" s="6">
+        <v>72.427999999999997</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13">
+        <v>177</v>
+      </c>
+      <c r="O13">
+        <v>0.43</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="2"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>30</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="2"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="2"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="2"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="1"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="2"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="1"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>34</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="2"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="1"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>35</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="2"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="1"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="I22" s="2"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="2"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>37</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="2"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>38</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="2"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="1"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>39</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="2"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="1"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -1223,7 +1430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1235,7 +1442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>